<commit_message>
2 approaches of reading data
</commit_message>
<xml_diff>
--- a/testSampleProj/DataFiles/TestData.xlsx
+++ b/testSampleProj/DataFiles/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\batch21SoftTest\testSampleProj\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A64D4FE-89B6-486E-A04E-9AC755B045F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFCAC6F-6903-4D58-8CC7-002B05AB4F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Salary</t>
+  </si>
+  <si>
+    <t>IsActive</t>
   </si>
 </sst>
 </file>
@@ -128,10 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,7 +431,7 @@
     <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -443,8 +447,11 @@
       <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -460,8 +467,11 @@
       <c r="E2" s="1">
         <v>23450</v>
       </c>
+      <c r="F2" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -477,8 +487,11 @@
       <c r="E3" s="1">
         <v>34567</v>
       </c>
+      <c r="F3" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -493,6 +506,9 @@
       </c>
       <c r="E4" s="1">
         <v>45678</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>